<commit_message>
Fixes for tests and scripts
</commit_message>
<xml_diff>
--- a/21-Spreads4Tests/QuadrupoleTriplet.xlsx
+++ b/21-Spreads4Tests/QuadrupoleTriplet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kennethlong/KL-GIT/CCAP/02-LhARA/04-LhARAlinearOptics/21-Spreads4Tests/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ken.long/KL-GIT/CCAP/02-LhARA/04-LhARAlinearOptics/21-Spreads4Tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F10A988-A484-ED49-BFB3-993C6F61D0A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B7B6397-85E8-2443-AC2E-E4CF50709287}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="57600" windowHeight="32400" activeTab="1" xr2:uid="{008B2FEE-BD6E-8742-A59F-ADD463C42F77}"/>
+    <workbookView xWindow="0" yWindow="640" windowWidth="30240" windowHeight="19000" activeTab="1" xr2:uid="{008B2FEE-BD6E-8742-A59F-ADD463C42F77}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1897,8 +1897,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DE99AEC-43F2-8D45-B0B0-4BCF34C0588E}">
   <dimension ref="A1:AQ48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="AF61" sqref="AF61"/>
+    <sheetView tabSelected="1" topLeftCell="R14" workbookViewId="0">
+      <selection activeCell="AC37" sqref="AC37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3422,6 +3422,20 @@
     <row r="24" spans="5:43" x14ac:dyDescent="0.2">
       <c r="U24" s="1"/>
     </row>
+    <row r="25" spans="5:43" x14ac:dyDescent="0.2">
+      <c r="F25">
+        <f>1/F19</f>
+        <v>-5.7845469216231321E-2</v>
+      </c>
+      <c r="V25">
+        <f>1/V19</f>
+        <v>3.3644969934764402E-3</v>
+      </c>
+      <c r="AL25">
+        <f>1/AL19</f>
+        <v>-5.7845469216231321E-2</v>
+      </c>
+    </row>
     <row r="27" spans="5:43" x14ac:dyDescent="0.2">
       <c r="AH27" s="47" t="s">
         <v>63</v>
@@ -4030,6 +4044,13 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="E1:K1"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="H10:J10"/>
+    <mergeCell ref="M2:O2"/>
+    <mergeCell ref="M10:O10"/>
+    <mergeCell ref="M1:S1"/>
     <mergeCell ref="AH27:AM27"/>
     <mergeCell ref="AA28:AF28"/>
     <mergeCell ref="T29:Y29"/>
@@ -4043,13 +4064,6 @@
     <mergeCell ref="AN10:AP10"/>
     <mergeCell ref="X10:Z10"/>
     <mergeCell ref="U1:AA1"/>
-    <mergeCell ref="E1:K1"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="E10:G10"/>
-    <mergeCell ref="H10:J10"/>
-    <mergeCell ref="M2:O2"/>
-    <mergeCell ref="M10:O10"/>
-    <mergeCell ref="M1:S1"/>
     <mergeCell ref="U2:W2"/>
     <mergeCell ref="U10:W10"/>
   </mergeCells>

</xml_diff>